<commit_message>
fix source framerowk names
</commit_message>
<xml_diff>
--- a/results/benchmarking/TVM-0.14.dev264-docker-19.02.2024.xlsx
+++ b/results/benchmarking/TVM-0.14.dev264-docker-19.02.2024.xlsx
@@ -263,14 +263,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1732,10 +1732,10 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1:K1"/>
+      <selection pane="bottomRight" activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,131 +1746,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4" t="s">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4" t="s">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4" t="s">
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" ht="72" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1903,10 +1903,10 @@
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1945,8 +1945,8 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1983,8 +1983,8 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
@@ -2021,8 +2021,8 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
@@ -2059,10 +2059,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -2101,8 +2101,8 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
@@ -2139,8 +2139,8 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
@@ -2177,8 +2177,8 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="2" t="s">
         <v>18</v>
       </c>
@@ -2215,10 +2215,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -2257,8 +2257,8 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="2" t="s">
         <v>23</v>
       </c>
@@ -2295,8 +2295,8 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="2" t="s">
         <v>24</v>
       </c>
@@ -2333,8 +2333,8 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="2" t="s">
         <v>25</v>
       </c>
@@ -2371,10 +2371,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -2413,8 +2413,8 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
       </c>
@@ -2451,8 +2451,8 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
       </c>
@@ -2489,8 +2489,8 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="2" t="s">
         <v>30</v>
       </c>
@@ -2527,10 +2527,10 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -2569,8 +2569,8 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2607,8 +2607,8 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2645,8 +2645,8 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
       <c r="D26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2683,10 +2683,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -2725,8 +2725,8 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
       <c r="D28" s="2" t="s">
         <v>35</v>
       </c>
@@ -2763,8 +2763,8 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
       <c r="D29" s="2" t="s">
         <v>36</v>
       </c>
@@ -2801,8 +2801,8 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
       <c r="D30" s="2" t="s">
         <v>37</v>
       </c>
@@ -2839,10 +2839,10 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -2881,8 +2881,8 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
       <c r="D32" s="2" t="s">
         <v>41</v>
       </c>
@@ -2919,8 +2919,8 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
       <c r="D33" s="2" t="s">
         <v>42</v>
       </c>
@@ -2957,8 +2957,8 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
       <c r="D34" s="2" t="s">
         <v>43</v>
       </c>
@@ -2995,11 +2995,11 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>32</v>
+      <c r="C35" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>45</v>
@@ -3037,8 +3037,8 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
       <c r="D36" s="2" t="s">
         <v>46</v>
       </c>
@@ -3075,8 +3075,8 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
       <c r="D37" s="2" t="s">
         <v>47</v>
       </c>
@@ -3113,8 +3113,8 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
       <c r="D38" s="2" t="s">
         <v>48</v>
       </c>
@@ -3151,11 +3151,11 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>32</v>
+      <c r="C39" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>45</v>
@@ -3193,8 +3193,8 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
       <c r="D40" s="2" t="s">
         <v>46</v>
       </c>
@@ -3231,8 +3231,8 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
       <c r="D41" s="2" t="s">
         <v>47</v>
       </c>
@@ -3269,8 +3269,8 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
       <c r="D42" s="2" t="s">
         <v>48</v>
       </c>
@@ -3307,10 +3307,10 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -3349,8 +3349,8 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
       <c r="D44" s="2" t="s">
         <v>46</v>
       </c>
@@ -3387,8 +3387,8 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
       <c r="D45" s="2" t="s">
         <v>47</v>
       </c>
@@ -3425,8 +3425,8 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
       <c r="D46" s="2" t="s">
         <v>48</v>
       </c>
@@ -3463,11 +3463,26 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="B1:B6"/>
+    <mergeCell ref="C1:C6"/>
+    <mergeCell ref="D1:D6"/>
+    <mergeCell ref="E1:E6"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="A7:A46"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="C7:C10"/>
@@ -3484,26 +3499,11 @@
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="C31:C34"/>
     <mergeCell ref="B35:B38"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A1:A6"/>
-    <mergeCell ref="B1:B6"/>
-    <mergeCell ref="C1:C6"/>
-    <mergeCell ref="D1:D6"/>
-    <mergeCell ref="E1:E6"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="C43:C46"/>
   </mergeCells>
   <conditionalFormatting sqref="A1">
     <cfRule type="notContainsBlanks" dxfId="63" priority="5">

</xml_diff>